<commit_message>
Refactor dataset processing and model evaluation scripts; update frame extraction logic and save validation data
</commit_message>
<xml_diff>
--- a/video_label_summary_val_metadata.xlsx
+++ b/video_label_summary_val_metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,19 +451,24 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>destruction</t>
+          <t>distracted</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>drowsy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>FPS</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dataset\val\videos\1080217202501_dms_drowsy_1.mp4</t>
+          <t>dataset/val\videos\1080217202501_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -478,689 +483,800 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dataset\val\videos\1120211202501_dms_drowsy_1.mp4</t>
+          <t>dataset/val\videos\1120211202501_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>271</v>
       </c>
       <c r="C3" t="n">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D3" t="n">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dataset\val\videos\1140217202501_dms_drowsy_5.mp4</t>
+          <t>dataset/val\videos\1140217202501_dms_drowsy_5.mp4</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_10.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_10.mp4</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>86</v>
       </c>
       <c r="C5" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_11.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_11.mp4</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>288</v>
       </c>
       <c r="C6" t="n">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="D6" t="n">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_12.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_12.mp4</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>288</v>
       </c>
       <c r="C7" t="n">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="D7" t="n">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_21.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_21.mp4</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>302</v>
       </c>
       <c r="C8" t="n">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D8" t="n">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="F8" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_22.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_22.mp4</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>307</v>
       </c>
       <c r="C9" t="n">
-        <v>104</v>
+        <v>169</v>
       </c>
       <c r="D9" t="n">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_24.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_24.mp4</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>283</v>
       </c>
       <c r="C10" t="n">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="D10" t="n">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_27.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_27.mp4</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>261</v>
       </c>
       <c r="C11" t="n">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D11" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_28.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_28.mp4</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>300</v>
       </c>
       <c r="C12" t="n">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="D12" t="n">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="F12" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_29.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_29.mp4</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>272</v>
       </c>
       <c r="C13" t="n">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D13" t="n">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E13" t="n">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_6.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_6.mp4</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>302</v>
       </c>
       <c r="C14" t="n">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="D14" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_7.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_7.mp4</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>307</v>
       </c>
       <c r="C15" t="n">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="D15" t="n">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_8.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_8.mp4</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>310</v>
       </c>
       <c r="C16" t="n">
-        <v>273</v>
+        <v>294</v>
       </c>
       <c r="D16" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>dataset\val\videos\270217202501_dms_drowsy_9.mp4</t>
+          <t>dataset/val\videos\270217202501_dms_drowsy_9.mp4</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>310</v>
       </c>
       <c r="C17" t="n">
-        <v>273</v>
+        <v>294</v>
       </c>
       <c r="D17" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>dataset\val\videos\3926989_dms_drowsy_1.mp4</t>
+          <t>dataset/val\videos\3926989_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>281</v>
       </c>
       <c r="C18" t="n">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="D18" t="n">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>dataset\val\videos\3927679_dms_drowsy_1.mp4</t>
+          <t>dataset/val\videos\3927679_dms_drowsy_1.mp4</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>293</v>
       </c>
       <c r="C19" t="n">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="D19" t="n">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F19" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_11.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_11.mp4</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>316</v>
       </c>
       <c r="C20" t="n">
-        <v>128</v>
+        <v>193</v>
       </c>
       <c r="D20" t="n">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_12.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_12.mp4</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>289</v>
       </c>
       <c r="C21" t="n">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="D21" t="n">
-        <v>139</v>
+        <v>77</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_2.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_2.mp4</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>326</v>
       </c>
       <c r="C22" t="n">
-        <v>251</v>
+        <v>311</v>
       </c>
       <c r="D22" t="n">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_3.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_3.mp4</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>283</v>
       </c>
       <c r="C23" t="n">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="D23" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_4.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_4.mp4</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>318</v>
       </c>
       <c r="C24" t="n">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="D24" t="n">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_5.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_5.mp4</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>304</v>
       </c>
       <c r="C25" t="n">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D25" t="n">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="F25" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_6.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_6.mp4</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>317</v>
       </c>
       <c r="C26" t="n">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="D26" t="n">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_7.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_7.mp4</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>295</v>
       </c>
       <c r="C27" t="n">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="D27" t="n">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="F27" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410217202501_dms_drowsy_9.mp4</t>
+          <t>dataset/val\videos\410217202501_dms_drowsy_9.mp4</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>329</v>
       </c>
       <c r="C28" t="n">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="D28" t="n">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410218202502_dms_drowsy_21.mp4</t>
+          <t>dataset/val\videos\410218202502_dms_drowsy_21.mp4</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>323</v>
       </c>
       <c r="C29" t="n">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_11.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_11.mp4</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>289</v>
       </c>
       <c r="C30" t="n">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="D30" t="n">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_12.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_12.mp4</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>289</v>
       </c>
       <c r="C31" t="n">
-        <v>222</v>
+        <v>251</v>
       </c>
       <c r="D31" t="n">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_13.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_13.mp4</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>321</v>
       </c>
       <c r="C32" t="n">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="D32" t="n">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_14.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_14.mp4</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>343</v>
       </c>
       <c r="C33" t="n">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="D33" t="n">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_15.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_15.mp4</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>240</v>
       </c>
       <c r="C34" t="n">
-        <v>86</v>
+        <v>143</v>
       </c>
       <c r="D34" t="n">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_16.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_16.mp4</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>240</v>
       </c>
       <c r="C35" t="n">
-        <v>86</v>
+        <v>143</v>
       </c>
       <c r="D35" t="n">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_2.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_2.mp4</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>331</v>
       </c>
       <c r="C36" t="n">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="D36" t="n">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_3.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_3.mp4</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>326</v>
       </c>
       <c r="C37" t="n">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D37" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>dataset\val\videos\410224202501_dms_drowsy_4.mp4</t>
+          <t>dataset/val\videos\410224202501_dms_drowsy_4.mp4</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>283</v>
       </c>
       <c r="C38" t="n">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="D38" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>